<commit_message>
feat: update invoices, cashflows, cashflow_categories
</commit_message>
<xml_diff>
--- a/public/template/template_customers.xlsx
+++ b/public/template/template_customers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93040dc21e0afcda/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Badru\Works\Fullstack\dashboard-intanet\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{5A78E546-5BC8-40A1-9778-A0A1D817D51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BCDFB5C-9A4D-4120-844A-DC513F41B174}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AE308A-99F3-41BC-B2A8-7626FC50E28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9EEEB96B-7EF4-4549-AFCE-12D37C2A317D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Jl. Cendramerta 1 RT: 03 RW: 05 Kel. Kota wetan Kec. Garut Kota Kab. Garut</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>24 Juni 2025</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>IDPEL-001</t>
+  </si>
+  <si>
+    <t>IDPEL-002</t>
+  </si>
+  <si>
+    <t>IDPEL-000</t>
+  </si>
+  <si>
+    <t>IDPEL-010</t>
   </si>
 </sst>
 </file>
@@ -190,11 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,10 +226,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,224 +525,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F2E6C1-B097-48A9-A4F1-0C0153AF3FBC}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1234567890123450</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>8123456789012</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="AH2" s="1"/>
+      <c r="L2" s="4">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1234567890123450</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>8123456789012</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>6</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="AH3" s="1"/>
+      <c r="L3" s="4">
+        <v>22</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1234567890123450</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>8123456789012</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="L4" s="4">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1234567890123450</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8123456789012</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>6</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="AH5" s="1"/>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1234567890123450</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>8123456789012</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="AH6" s="1"/>
+      <c r="L6" s="4">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="AI6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>